<commit_message>
Data Envelopemnt Analysis For Two Input And One Output
</commit_message>
<xml_diff>
--- a/DataEnvelopmentAnalysisTwoInputAndOneOutput.xlsx
+++ b/DataEnvelopmentAnalysisTwoInputAndOneOutput.xlsx
@@ -4,188 +4,190 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="LP1" sheetId="1" r:id="rId1"/>
-    <sheet name="LP2" sheetId="2" r:id="rId2"/>
-    <sheet name="LP3" sheetId="3" r:id="rId3"/>
-    <sheet name="LP4" sheetId="4" r:id="rId4"/>
-    <sheet name="LP5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sensitivity Report 1" sheetId="6" r:id="rId1"/>
+    <sheet name="LP1" sheetId="1" r:id="rId2"/>
+    <sheet name="LP2" sheetId="2" r:id="rId3"/>
+    <sheet name="LP3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sensitivity Report 4" sheetId="7" r:id="rId5"/>
+    <sheet name="LP4" sheetId="4" r:id="rId6"/>
+    <sheet name="LP5" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'LP1'!$G$5:$I$5</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">'LP2'!$G$5:$I$5</definedName>
-    <definedName name="solver_adj" localSheetId="2" hidden="1">'LP3'!$G$5:$I$5</definedName>
-    <definedName name="solver_adj" localSheetId="3" hidden="1">'LP4'!$G$5:$I$5</definedName>
-    <definedName name="solver_adj" localSheetId="4" hidden="1">'LP5'!$G$5:$I$5</definedName>
-    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'LP1'!$G$5:$I$5</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'LP2'!$G$5:$I$5</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">'LP3'!$G$5:$I$5</definedName>
+    <definedName name="solver_adj" localSheetId="5" hidden="1">'LP4'!$G$5:$I$5</definedName>
+    <definedName name="solver_adj" localSheetId="6" hidden="1">'LP5'!$G$5:$I$5</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
-    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_cvg" localSheetId="5" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_eng" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_est" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'LP1'!$H$10</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'LP2'!$H$10</definedName>
-    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'LP3'!$H$10</definedName>
-    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'LP4'!$H$10</definedName>
-    <definedName name="solver_lhs1" localSheetId="4" hidden="1">'LP5'!$H$10</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'LP1'!$H$12:$H$16</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'LP2'!$H$12:$H$16</definedName>
-    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'LP3'!$H$12:$H$16</definedName>
-    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'LP4'!$H$12:$H$16</definedName>
-    <definedName name="solver_lhs2" localSheetId="4" hidden="1">'LP5'!$H$12:$H$16</definedName>
-    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'LP1'!$H$10</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'LP2'!$H$10</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'LP3'!$H$10</definedName>
+    <definedName name="solver_lhs1" localSheetId="5" hidden="1">'LP4'!$H$10</definedName>
+    <definedName name="solver_lhs1" localSheetId="6" hidden="1">'LP5'!$H$10</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'LP1'!$H$12:$H$16</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'LP2'!$H$12:$H$16</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'LP3'!$H$12:$H$16</definedName>
+    <definedName name="solver_lhs2" localSheetId="5" hidden="1">'LP4'!$H$12:$H$16</definedName>
+    <definedName name="solver_lhs2" localSheetId="6" hidden="1">'LP5'!$H$12:$H$16</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mip" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
-    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mni" localSheetId="5" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
-    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_mrt" localSheetId="5" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_msl" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_neg" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_nod" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_num" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'LP1'!$J$7</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">'LP2'!$J$7</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">'LP3'!$J$7</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">'LP4'!$J$7</definedName>
-    <definedName name="solver_opt" localSheetId="4" hidden="1">'LP5'!$J$7</definedName>
-    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_nwt" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'LP1'!$J$7</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'LP2'!$J$7</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">'LP3'!$J$7</definedName>
+    <definedName name="solver_opt" localSheetId="5" hidden="1">'LP4'!$J$7</definedName>
+    <definedName name="solver_opt" localSheetId="6" hidden="1">'LP5'!$J$7</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
-    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rbv" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_pre" localSheetId="5" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="6" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rel1" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'LP1'!$J$10</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'LP2'!$J$10</definedName>
-    <definedName name="solver_rhs1" localSheetId="2" hidden="1">'LP3'!$J$10</definedName>
-    <definedName name="solver_rhs1" localSheetId="3" hidden="1">'LP4'!$J$10</definedName>
-    <definedName name="solver_rhs1" localSheetId="4" hidden="1">'LP5'!$J$10</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'LP1'!$J$12:$J$16</definedName>
-    <definedName name="solver_rhs2" localSheetId="1" hidden="1">'LP2'!$J$12:$J$16</definedName>
-    <definedName name="solver_rhs2" localSheetId="2" hidden="1">'LP3'!$J$12:$J$16</definedName>
-    <definedName name="solver_rhs2" localSheetId="3" hidden="1">'LP4'!$J$12:$J$16</definedName>
-    <definedName name="solver_rhs2" localSheetId="4" hidden="1">'LP5'!$J$12:$J$16</definedName>
-    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'LP1'!$J$10</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">'LP2'!$J$10</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">'LP3'!$J$10</definedName>
+    <definedName name="solver_rhs1" localSheetId="5" hidden="1">'LP4'!$J$10</definedName>
+    <definedName name="solver_rhs1" localSheetId="6" hidden="1">'LP5'!$J$10</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">'LP1'!$J$12:$J$16</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">'LP2'!$J$12:$J$16</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">'LP3'!$J$12:$J$16</definedName>
+    <definedName name="solver_rhs2" localSheetId="5" hidden="1">'LP4'!$J$12:$J$16</definedName>
+    <definedName name="solver_rhs2" localSheetId="6" hidden="1">'LP5'!$J$12:$J$16</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rsd" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
-    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_ssz" localSheetId="5" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tim" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
-    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_tol" localSheetId="5" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_typ" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="64">
   <si>
     <t>Sales Office</t>
   </si>
@@ -266,13 +268,124 @@
   </si>
   <si>
     <t>y15</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 15.0 Sensitivity Report</t>
+  </si>
+  <si>
+    <t>Worksheet: [DataEnvelopmentAnalysisTwoInputAndOneOutput.xlsx]LP1</t>
+  </si>
+  <si>
+    <t>Report Created: 28-04-2024 00:03:20</t>
+  </si>
+  <si>
+    <t>Variable Cells</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Reduced</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
+    <t>Allowable</t>
+  </si>
+  <si>
+    <t>Increase</t>
+  </si>
+  <si>
+    <t>Decrease</t>
+  </si>
+  <si>
+    <t>Constraints</t>
+  </si>
+  <si>
+    <t>Shadow</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Constraint</t>
+  </si>
+  <si>
+    <t>R.H. Side</t>
+  </si>
+  <si>
+    <t>$G$5</t>
+  </si>
+  <si>
+    <t>$H$5</t>
+  </si>
+  <si>
+    <t>$I$5</t>
+  </si>
+  <si>
+    <t>$H$10</t>
+  </si>
+  <si>
+    <t>$H$12</t>
+  </si>
+  <si>
+    <t>$H$13</t>
+  </si>
+  <si>
+    <t>$H$14</t>
+  </si>
+  <si>
+    <t>$H$15</t>
+  </si>
+  <si>
+    <t>$H$16</t>
+  </si>
+  <si>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>2 and 5</t>
+  </si>
+  <si>
+    <t>DMU2</t>
+  </si>
+  <si>
+    <t>DMU5</t>
+  </si>
+  <si>
+    <t>Worksheet: [DataEnvelopmentAnalysisTwoInputAndOneOutput.xlsx]LP4</t>
+  </si>
+  <si>
+    <t>Report Created: 28-04-2024 00:19:22</t>
+  </si>
+  <si>
+    <t>2 and 3</t>
+  </si>
+  <si>
+    <t>DMU3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,16 +393,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -297,12 +432,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,10 +790,355 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="2.1796875" customWidth="1"/>
+    <col min="2" max="2" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2.0635575732562941E-6</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>138076.92307692306</v>
+      </c>
+      <c r="H9" s="2">
+        <v>48307.692307692327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2.9302517540239364E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2.0933333333333342</v>
+      </c>
+      <c r="H10" s="2">
+        <v>5.9833333333333325</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3">
+        <v>7.919933966157655E-7</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1E+30</v>
+      </c>
+      <c r="H11" s="3">
+        <v>999999.99999999988</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.79199339661576551</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1E+30</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.79199339661576551</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1E+30</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.20800660338423446</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.79199339661576551</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.74081716879900938</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.17401129943502833</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.23666666666666658</v>
+      </c>
+      <c r="J18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.79199339661576551</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1E+30</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.4449030127940572</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.79199339661576551</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1E+30</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.30581923235658293</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.79199339661576551</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.25918283120099062</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.23666666666666658</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.28579003181336177</v>
+      </c>
+      <c r="J21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -620,12 +1148,18 @@
     <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="M1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -633,7 +1167,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G3" t="s">
         <v>10</v>
       </c>
@@ -644,7 +1178,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -664,7 +1198,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>1</v>
       </c>
@@ -684,7 +1218,7 @@
         <v>7.919933966157655E-7</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>2</v>
       </c>
@@ -695,7 +1229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>3</v>
       </c>
@@ -716,7 +1250,7 @@
         <v>0.79199339661576551</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>4</v>
       </c>
@@ -727,7 +1261,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>5</v>
       </c>
@@ -738,7 +1272,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="H10">
         <f>SUMPRODUCT(C5:D5,G5:H5)</f>
         <v>1</v>
@@ -750,7 +1284,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G12">
+        <v>1</v>
+      </c>
       <c r="H12">
         <f>$B$2*$I$5</f>
         <v>0.79199339661576551</v>
@@ -763,7 +1300,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G13" s="6">
+        <v>2</v>
+      </c>
       <c r="H13">
         <f t="shared" ref="H13:H16" si="0">$B$2*$I$5</f>
         <v>0.79199339661576551</v>
@@ -776,7 +1316,10 @@
         <v>0.79199339661576551</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G14">
+        <v>3</v>
+      </c>
       <c r="H14">
         <f t="shared" si="0"/>
         <v>0.79199339661576551</v>
@@ -789,7 +1332,10 @@
         <v>1.2368964094098227</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G15">
+        <v>4</v>
+      </c>
       <c r="H15">
         <f t="shared" si="0"/>
         <v>0.79199339661576551</v>
@@ -802,7 +1348,10 @@
         <v>1.0978126289723484</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G16" s="6">
+        <v>5</v>
+      </c>
       <c r="H16">
         <f t="shared" si="0"/>
         <v>0.79199339661576551</v>
@@ -813,221 +1362,6 @@
       <c r="J16">
         <f t="shared" si="1"/>
         <v>0.79199339661576551</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>300000</v>
-      </c>
-      <c r="D5">
-        <v>13</v>
-      </c>
-      <c r="G5">
-        <v>2.6055237102657635E-6</v>
-      </c>
-      <c r="H5">
-        <v>3.6998436685773836E-2</v>
-      </c>
-      <c r="I5">
-        <v>9.9999999999999995E-7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>256000</v>
-      </c>
-      <c r="D6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>500000</v>
-      </c>
-      <c r="D7">
-        <v>7</v>
-      </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7">
-        <f>B2*I5</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>390000</v>
-      </c>
-      <c r="D8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>185000</v>
-      </c>
-      <c r="D9">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H10">
-        <f>SUMPRODUCT(C6:D6,G5:H5)</f>
-        <v>1</v>
-      </c>
-      <c r="I10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H12">
-        <f>$B$2*$I$5</f>
-        <v>1</v>
-      </c>
-      <c r="I12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12">
-        <f>SUMPRODUCT($G$5:$H$5,C5:D5)</f>
-        <v>1.262636789994789</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H13">
-        <f t="shared" ref="H13:H16" si="0">$B$2*$I$5</f>
-        <v>1</v>
-      </c>
-      <c r="I13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13">
-        <f t="shared" ref="J13:J16" si="1">SUMPRODUCT($G$5:$H$5,C6:D6)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="1"/>
-        <v>1.5617509119332986</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I15" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="1"/>
-        <v>1.386138613861386</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I16" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="1"/>
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1065,13 +1399,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -1105,13 +1439,13 @@
         <v>13</v>
       </c>
       <c r="G5">
-        <v>7.3855243722304268E-7</v>
+        <v>2.6055237102657635E-6</v>
       </c>
       <c r="H5">
-        <v>9.0103397341211228E-2</v>
+        <v>3.6998436685773836E-2</v>
       </c>
       <c r="I5">
-        <v>1.0000000000000002E-6</v>
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1143,7 +1477,7 @@
       </c>
       <c r="J7">
         <f>B2*I5</f>
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -1170,7 +1504,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H10">
-        <f>SUMPRODUCT(C7:D7,G5:H5)</f>
+        <f>SUMPRODUCT(C6:D6,G5:H5)</f>
         <v>1</v>
       </c>
       <c r="I10" t="s">
@@ -1183,20 +1517,20 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H12">
         <f>$B$2*$I$5</f>
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="I12" t="s">
         <v>14</v>
       </c>
       <c r="J12">
         <f>SUMPRODUCT($G$5:$H$5,C5:D5)</f>
-        <v>1.3929098966026587</v>
+        <v>1.262636789994789</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H13">
         <f t="shared" ref="H13:H16" si="0">$B$2*$I$5</f>
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="I13" t="s">
         <v>14</v>
@@ -1209,40 +1543,40 @@
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="I14" t="s">
         <v>14</v>
       </c>
       <c r="J14">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.5617509119332986</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="I15" t="s">
         <v>14</v>
       </c>
       <c r="J15">
         <f t="shared" si="1"/>
-        <v>1.1890694239290989</v>
+        <v>1.386138613861386</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="I16" t="s">
         <v>14</v>
       </c>
       <c r="J16">
         <f t="shared" si="1"/>
-        <v>1.3980797636632201</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1255,7 +1589,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1280,13 +1614,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -1320,13 +1654,13 @@
         <v>13</v>
       </c>
       <c r="G5">
-        <v>6.2111801242236047E-7</v>
+        <v>7.3855243722304268E-7</v>
       </c>
       <c r="H5">
-        <v>7.5776397515527935E-2</v>
+        <v>9.0103397341211228E-2</v>
       </c>
       <c r="I5">
-        <v>8.4099378881987579E-7</v>
+        <v>1.0000000000000002E-6</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1358,7 +1692,7 @@
       </c>
       <c r="J7">
         <f>B2*I5</f>
-        <v>0.84099378881987574</v>
+        <v>1.0000000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -1385,7 +1719,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H10">
-        <f>SUMPRODUCT(C8:D8,G5:H5)</f>
+        <f>SUMPRODUCT(C7:D7,G5:H5)</f>
         <v>1</v>
       </c>
       <c r="I10" t="s">
@@ -1398,66 +1732,66 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H12">
         <f>$B$2*$I$5</f>
-        <v>0.84099378881987574</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I12" t="s">
         <v>14</v>
       </c>
       <c r="J12">
         <f>SUMPRODUCT($G$5:$H$5,C5:D5)</f>
-        <v>1.1714285714285713</v>
+        <v>1.3929098966026587</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H13">
         <f t="shared" ref="H13:H16" si="0">$B$2*$I$5</f>
-        <v>0.84099378881987574</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I13" t="s">
         <v>14</v>
       </c>
       <c r="J13">
         <f t="shared" ref="J13:J16" si="1">SUMPRODUCT($G$5:$H$5,C6:D6)</f>
-        <v>0.84099378881987563</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>0.84099378881987574</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I14" t="s">
         <v>14</v>
       </c>
       <c r="J14">
         <f t="shared" si="1"/>
-        <v>0.84099378881987574</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>0.84099378881987574</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I15" t="s">
         <v>14</v>
       </c>
       <c r="J15">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.1890694239290989</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>0.84099378881987574</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="I16" t="s">
         <v>14</v>
       </c>
       <c r="J16">
         <f t="shared" si="1"/>
-        <v>1.1757763975155278</v>
+        <v>1.3980797636632201</v>
       </c>
     </row>
   </sheetData>
@@ -1467,10 +1801,591 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="2.1796875" customWidth="1"/>
+    <col min="2" max="2" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>6.2111801242236047E-7</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>95000</v>
+      </c>
+      <c r="H9" s="2">
+        <v>227000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2">
+        <v>7.5776397515527935E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5.8205128205128194</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2.4358974358974357</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3">
+        <v>8.4099378881987579E-7</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1E+30</v>
+      </c>
+      <c r="H11" s="3">
+        <v>999999.99999999965</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.84099378881987574</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1E+30</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.84099378881987574</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1E+30</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.33043478260869563</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.84099378881987574</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.70496894409937882</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.18333333333333326</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.20000000000000009</v>
+      </c>
+      <c r="J18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.84099378881987574</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.29503105590062112</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.20000000000000007</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.40526315789473671</v>
+      </c>
+      <c r="J19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.84099378881987574</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1E+30</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.15900621118012426</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.84099378881987574</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1E+30</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.33478260869565202</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>300000</v>
+      </c>
+      <c r="D5">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>6.2111801242236047E-7</v>
+      </c>
+      <c r="H5">
+        <v>7.5776397515527935E-2</v>
+      </c>
+      <c r="I5">
+        <v>8.4099378881987579E-7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>256000</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>500000</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7">
+        <f>B2*I5</f>
+        <v>0.84099378881987574</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>390000</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>185000</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H10">
+        <f>SUMPRODUCT(C8:D8,G5:H5)</f>
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <f>$B$2*$I$5</f>
+        <v>0.84099378881987574</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12">
+        <f>SUMPRODUCT($G$5:$H$5,C5:D5)</f>
+        <v>1.1714285714285713</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G13" s="6">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ref="H13:H16" si="0">$B$2*$I$5</f>
+        <v>0.84099378881987574</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ref="J13:J16" si="1">SUMPRODUCT($G$5:$H$5,C6:D6)</f>
+        <v>0.84099378881987563</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G14" s="6">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0.84099378881987574</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>0.84099378881987574</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>0.84099378881987574</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>0.84099378881987574</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>1.1757763975155278</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>